<commit_message>
publication and ballot push
</commit_message>
<xml_diff>
--- a/Dec 2013 Tracker.xlsx
+++ b/Dec 2013 Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>vMR LM DSTU ballot</t>
   </si>
@@ -54,7 +54,16 @@
     <t>vMR XML Informative pub</t>
   </si>
   <si>
-    <t>Provided to Paul Wed AM</t>
+    <t>Submitted to Don Thurs AM</t>
+  </si>
+  <si>
+    <t>Submitted to Don Thurs AM by ITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ready to submit </t>
+  </si>
+  <si>
+    <t>Ready to submit after peer review</t>
   </si>
 </sst>
 </file>
@@ -405,13 +414,13 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,16 +443,25 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -457,20 +475,32 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>